<commit_message>
implementado validador de telas e cadastro completo
</commit_message>
<xml_diff>
--- a/build-cibapp-Desktop_Qt_5_13_0_MinGW_32_bit-Release/Laboratorio.xlsx
+++ b/build-cibapp-Desktop_Qt_5_13_0_MinGW_32_bit-Release/Laboratorio.xlsx
@@ -11,6 +11,89 @@
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+  <si>
+    <t>01/01/2000</t>
+  </si>
+  <si>
+    <t>tryjrtyjrtyjrtyjrt</t>
+  </si>
+  <si>
+    <t>AgroIndústria</t>
+  </si>
+  <si>
+    <t>Codigestão</t>
+  </si>
+  <si>
+    <t>Abatedouro de aves</t>
+  </si>
+  <si>
+    <t>Água residual</t>
+  </si>
+  <si>
+    <t>rthsrhtytjtj</t>
+  </si>
+  <si>
+    <t>thrsrhs</t>
+  </si>
+  <si>
+    <t>Protocolo</t>
+  </si>
+  <si>
+    <t>Coleta</t>
+  </si>
+  <si>
+    <t>argaergaegr argaergaegr argaergaegrargaergaegr argaergaegr argaergaegr argaergaegr argaergaegr argaergaegr</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -332,4 +415,117 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V2" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageSetup/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
gerado release 3 e realizando testes com laboratorio
</commit_message>
<xml_diff>
--- a/build-cibapp-Desktop_Qt_5_13_0_MinGW_32_bit-Release/Laboratorio.xlsx
+++ b/build-cibapp-Desktop_Qt_5_13_0_MinGW_32_bit-Release/Laboratorio.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>01/01/2000</t>
   </si>
@@ -92,6 +92,45 @@
   </si>
   <si>
     <t>21</t>
+  </si>
+  <si>
+    <t>wefwfwf</t>
+  </si>
+  <si>
+    <t>wefwf</t>
+  </si>
+  <si>
+    <t>wefwfwfw</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>ragagegtrbbr</t>
+  </si>
+  <si>
+    <t>Resíduo urbano</t>
+  </si>
+  <si>
+    <t>Resíduos alimentares</t>
+  </si>
+  <si>
+    <t>Cebola</t>
+  </si>
+  <si>
+    <t>Amostra suco</t>
+  </si>
+  <si>
+    <t>wergwergwerg</t>
+  </si>
+  <si>
+    <t>wergrtrtrt</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>1234124</t>
   </si>
 </sst>
 </file>
@@ -419,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -525,6 +564,148 @@
         <v>25</v>
       </c>
     </row>
+    <row r="3" spans="1:23">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageSetup/>
 </worksheet>

</xml_diff>

<commit_message>
iniciado nova implementacao com header
</commit_message>
<xml_diff>
--- a/build-cibapp-Desktop_Qt_5_13_0_MinGW_32_bit-Release/Laboratorio.xlsx
+++ b/build-cibapp-Desktop_Qt_5_13_0_MinGW_32_bit-Release/Laboratorio.xlsx
@@ -14,123 +14,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
-  <si>
-    <t>01/01/2000</t>
-  </si>
-  <si>
-    <t>tryjrtyjrtyjrtyjrt</t>
-  </si>
-  <si>
-    <t>AgroIndústria</t>
-  </si>
-  <si>
-    <t>Codigestão</t>
-  </si>
-  <si>
-    <t>Abatedouro de aves</t>
-  </si>
-  <si>
-    <t>Água residual</t>
-  </si>
-  <si>
-    <t>rthsrhtytjtj</t>
-  </si>
-  <si>
-    <t>thrsrhs</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+  <si>
+    <t>Data de incubação</t>
   </si>
   <si>
     <t>Protocolo</t>
   </si>
   <si>
-    <t>Coleta</t>
-  </si>
-  <si>
-    <t>argaergaegr argaergaegr argaergaegrargaergaegr argaergaegr argaergaegr argaergaegr argaergaegr argaergaegr</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>wefwfwf</t>
-  </si>
-  <si>
-    <t>wefwf</t>
-  </si>
-  <si>
-    <t>wefwfwfw</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>ragagegtrbbr</t>
-  </si>
-  <si>
-    <t>Resíduo urbano</t>
-  </si>
-  <si>
-    <t>Resíduos alimentares</t>
-  </si>
-  <si>
-    <t>Cebola</t>
-  </si>
-  <si>
-    <t>Amostra suco</t>
-  </si>
-  <si>
-    <t>wergwergwerg</t>
-  </si>
-  <si>
-    <t>wergrtrtrt</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>1234124</t>
+    <t>Procedência</t>
+  </si>
+  <si>
+    <t>Mercado</t>
+  </si>
+  <si>
+    <t>Origem matéria-prima</t>
+  </si>
+  <si>
+    <t>Setor</t>
+  </si>
+  <si>
+    <t>Amostra/fase</t>
+  </si>
+  <si>
+    <t>Ponto de coleta</t>
+  </si>
+  <si>
+    <t>Informações complementares</t>
+  </si>
+  <si>
+    <t>Biogás (LNbiogás.kg sv¹)</t>
+  </si>
+  <si>
+    <t>Maior e menor</t>
+  </si>
+  <si>
+    <t>Critério de aceitação</t>
+  </si>
+  <si>
+    <t>Metano (LNbiogás.kg sv¹)</t>
+  </si>
+  <si>
+    <t>Metano (LNCH4.kg¹ sv)</t>
+  </si>
+  <si>
+    <t>% de Metano no Biogás</t>
+  </si>
+  <si>
+    <t>ST (%)</t>
+  </si>
+  <si>
+    <t>Sólidos totais (g/kg)</t>
+  </si>
+  <si>
+    <t>SV (%)</t>
+  </si>
+  <si>
+    <t>Sólidos voláteis (g/kg)</t>
+  </si>
+  <si>
+    <t>SF (%)</t>
+  </si>
+  <si>
+    <t>DQO(mg de O2/L)</t>
+  </si>
+  <si>
+    <t>pH</t>
   </si>
 </sst>
 </file>
@@ -458,13 +407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,220 +439,67 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="N2" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="O2" t="s">
+      <c r="U1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="P2" t="s">
+      <c r="W1" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="X1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="R2" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AA1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
-      <c r="T2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U2" t="s">
-        <v>23</v>
-      </c>
-      <c r="V2" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S3" t="s">
-        <v>29</v>
-      </c>
-      <c r="T3" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" t="s">
-        <v>29</v>
-      </c>
-      <c r="V3" t="s">
-        <v>29</v>
-      </c>
-      <c r="W3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V4" t="s">
-        <v>29</v>
-      </c>
-      <c r="W4" t="s">
-        <v>29</v>
+      <c r="AC1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>